<commit_message>
removed RT exp. yields; added SC ones
</commit_message>
<xml_diff>
--- a/application/input/prod_mw.xlsx
+++ b/application/input/prod_mw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejm6426/Documents/scRBA/application/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790B62EB-7B76-0143-AAC4-51DC1350F4F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BA78A3-2808-1742-96D6-5D4C5BBAAA23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13680" yWindow="860" windowWidth="16560" windowHeight="17280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -4081,9 +4081,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="108" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15"/>
@@ -4149,6 +4149,9 @@
       <c r="D2">
         <v>256.39999999999998</v>
       </c>
+      <c r="E2">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="3" spans="1:11" ht="16">
       <c r="A3" t="s">
@@ -4163,6 +4166,9 @@
       <c r="D3">
         <v>242.44</v>
       </c>
+      <c r="E3">
+        <v>5.0000000000000001E-3</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="16">
       <c r="A4" t="s">
@@ -4177,6 +4183,9 @@
       <c r="D4">
         <v>74.12</v>
       </c>
+      <c r="E4">
+        <v>0.04</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="16">
       <c r="A5" t="s">
@@ -4192,10 +4201,7 @@
         <v>824.3</v>
       </c>
       <c r="E5">
-        <v>0.129384</v>
-      </c>
-      <c r="F5">
-        <v>0.14680000000000001</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="G5" t="s">
         <v>447</v>
@@ -4234,6 +4240,9 @@
       <c r="D7">
         <v>103.1</v>
       </c>
+      <c r="E7">
+        <v>0.13</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="16">
       <c r="A8" t="s">
@@ -4276,6 +4285,9 @@
       <c r="D10">
         <v>246.3</v>
       </c>
+      <c r="E10">
+        <v>3.0000000000000001E-3</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="16">
       <c r="A11" t="s">
@@ -4290,6 +4302,9 @@
       <c r="D11">
         <v>46.07</v>
       </c>
+      <c r="E11">
+        <v>0.44</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="16">
       <c r="A12" t="s">
@@ -4304,6 +4319,9 @@
       <c r="D12">
         <v>89.07</v>
       </c>
+      <c r="E12">
+        <v>0.69</v>
+      </c>
     </row>
     <row r="13" spans="1:11" ht="16">
       <c r="A13" t="s">
@@ -4318,6 +4336,9 @@
       <c r="D13">
         <v>90.12</v>
       </c>
+      <c r="E13">
+        <v>0.11</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="16">
       <c r="A14" t="s">
@@ -4332,6 +4353,9 @@
       <c r="D14">
         <v>74.12</v>
       </c>
+      <c r="E14">
+        <v>0.06</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="16">
       <c r="A15" t="s">
@@ -4346,6 +4370,9 @@
       <c r="D15">
         <v>90.08</v>
       </c>
+      <c r="E15">
+        <v>0.13</v>
+      </c>
     </row>
     <row r="16" spans="1:11" ht="16">
       <c r="A16" t="s">
@@ -4360,6 +4387,9 @@
       <c r="D16">
         <v>90.08</v>
       </c>
+      <c r="E16">
+        <v>0.14000000000000001</v>
+      </c>
     </row>
     <row r="17" spans="1:16" ht="16">
       <c r="A17" t="s">
@@ -4374,6 +4404,9 @@
       <c r="D17">
         <v>116.07</v>
       </c>
+      <c r="E17">
+        <v>0.11</v>
+      </c>
     </row>
     <row r="18" spans="1:16" ht="16">
       <c r="A18" t="s">
@@ -4388,6 +4421,9 @@
       <c r="D18">
         <v>132.07</v>
       </c>
+      <c r="E18">
+        <v>0.31</v>
+      </c>
     </row>
     <row r="19" spans="1:16" ht="16">
       <c r="A19" t="s">
@@ -4416,6 +4452,9 @@
       <c r="D20">
         <v>140.09</v>
       </c>
+      <c r="E20">
+        <v>7.0000000000000007E-2</v>
+      </c>
     </row>
     <row r="21" spans="1:16" ht="16">
       <c r="A21" t="s">
@@ -4430,6 +4469,9 @@
       <c r="D21">
         <v>137.11000000000001</v>
       </c>
+      <c r="E21">
+        <v>7.0000000000000007E-2</v>
+      </c>
     </row>
     <row r="22" spans="1:16" ht="16">
       <c r="A22" t="s">
@@ -4444,6 +4486,9 @@
       <c r="D22">
         <v>137.13999999999999</v>
       </c>
+      <c r="E22">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="23" spans="1:16" ht="16">
       <c r="A23" t="s">
@@ -4458,6 +4503,9 @@
       <c r="D23">
         <v>122.16</v>
       </c>
+      <c r="E23">
+        <v>0.08</v>
+      </c>
     </row>
     <row r="24" spans="1:16" ht="16">
       <c r="A24" t="s">
@@ -4472,6 +4520,9 @@
       <c r="D24">
         <v>163.15</v>
       </c>
+      <c r="E24">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="25" spans="1:16" ht="16">
       <c r="A25" t="s">
@@ -4486,6 +4537,9 @@
       <c r="D25">
         <v>228.24</v>
       </c>
+      <c r="E25">
+        <v>2.0000000000000001E-4</v>
+      </c>
     </row>
     <row r="26" spans="1:16" ht="16">
       <c r="A26" t="s">
@@ -4500,6 +4554,9 @@
       <c r="D26">
         <v>104.15</v>
       </c>
+      <c r="E26">
+        <v>1E-3</v>
+      </c>
     </row>
     <row r="27" spans="1:16" ht="16">
       <c r="A27" t="s">
@@ -4528,6 +4585,9 @@
       <c r="D28">
         <v>92.09</v>
       </c>
+      <c r="E28">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="29" spans="1:16" ht="16">
       <c r="A29" t="s">
@@ -4557,12 +4617,6 @@
       <c r="D30">
         <v>126.11004</v>
       </c>
-      <c r="E30">
-        <v>0.11450973051259666</v>
-      </c>
-      <c r="F30">
-        <v>0.1208420658404822</v>
-      </c>
       <c r="G30" t="s">
         <v>445</v>
       </c>
@@ -4598,14 +4652,6 @@
       <c r="D31">
         <v>268.5</v>
       </c>
-      <c r="E31">
-        <f>0.04*0.68</f>
-        <v>2.7200000000000002E-2</v>
-      </c>
-      <c r="F31">
-        <f>0.04*0.7</f>
-        <v>2.7999999999999997E-2</v>
-      </c>
       <c r="G31" t="s">
         <v>446</v>
       </c>
@@ -4651,14 +4697,6 @@
       <c r="D32">
         <v>270.5</v>
       </c>
-      <c r="E32">
-        <f>0.04*0.15</f>
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="F32">
-        <f>0.04*0.23</f>
-        <v>9.1999999999999998E-3</v>
-      </c>
       <c r="G32" t="str">
         <f>G31</f>
         <v>media:reset;c_sources:EX_sucr_e;media:reset;c_sources:EX_sucr_e;EX_sucr_e:(-0.332925,1000);EX_k_e:(-0.1,1000);EX_nh4_e:(-0.09,1000);EX_ca2_e:(-0.002844,1000);EX_mg2_e:(-0.004689,1000);EX_pi_e:(-0.01,1000);EX_no3_e:(-0.003217,1000);EX_cl_e:(-0.00643,1000);EX_so4_e:(-0.002,1000);EX_h_e:(-1000,1000);EX_h2o_e:(-1000,1000);EX_btn_c:(-0.01,1000);EX_o2_e:(-26.25403530509562,1000);EX_co2_e:(0,1000);EX_thm_e:(-1000,1000);EX_ribflv_e:(-1000,1000);EX_nac_e:(-1000,1000);EX_pydxn_e:(-1000,1000);EX_fol_e:(-1000,1000);EX_pnto__R_e:(-1000,1000);EX_4abz_e:(-1000,1000);EX_cu2_e:(-1000,1000);EX_fe2_e:(-1000,1000);EX_fe3_e:(-1000,1000);EX_mn2_e:(-1000,1000);EX_na1_e:(-1000,1000);EX_ni2_e:(-1000,1000);EX_zn2_e:(-1000,1000);EX_cobalt2_e:(-1000,1000);EX_inost_e:(-1000,1000);EX_asp__L_e:(-0.00046,1000);EX_thr__L_e:(-0.000276,1000);EX_ser__L_e:(-0.000334,1000);EX_glu__L_e:(-0.001013,1000);EX_gly_e:(-0.000747,1000);EX_tyr__L_e:(-0.000094,1000);EX_lys__L_e:(-0.000216,1000);EX_arg__L_e:(-0.000236,1000);EX_trp__L_e:(-0.000023,1000);EX_chol_e:(-0.090319,1000);EX_ala__L_e:(-0.001179,1000);EX_val__L_e:(-0.000463,1000);EX_met__L_e:(-0.000132,1000);EX_ile__L_e:(-0.000253,1000);EX_leu__L_e:(-0.000709,1000);EX_phe__L_e:(-0.000229,1000);EX_his__L_e:(-0.000205,1000);EX_pro__L_e:(-0.000761,1000);BIOMASS_AERO_SC_hvd:(0.0133333333333333,1000)</v>
@@ -4690,14 +4728,6 @@
       </c>
       <c r="D33">
         <v>242.44</v>
-      </c>
-      <c r="E33">
-        <f>0.04*0.09</f>
-        <v>3.5999999999999999E-3</v>
-      </c>
-      <c r="F33">
-        <f>0.04*0.15</f>
-        <v>6.0000000000000001E-3</v>
       </c>
       <c r="G33" t="str">
         <f>G32</f>
@@ -4853,7 +4883,7 @@
       <c r="AF2"/>
       <c r="AG2"/>
     </row>
-    <row r="3" spans="1:36" s="23" customFormat="1" ht="46">
+    <row r="3" spans="1:36" s="23" customFormat="1" ht="48">
       <c r="A3" s="21" t="s">
         <v>139</v>
       </c>
@@ -7605,7 +7635,7 @@
       <c r="AF2"/>
       <c r="AG2"/>
     </row>
-    <row r="3" spans="1:36" s="23" customFormat="1" ht="46">
+    <row r="3" spans="1:36" s="23" customFormat="1" ht="48">
       <c r="A3" s="21" t="s">
         <v>139</v>
       </c>

</xml_diff>